<commit_message>
aas changed to adn
</commit_message>
<xml_diff>
--- a/site_audit/url-change-history.xlsx
+++ b/site_audit/url-change-history.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\old_site_projects\site_audit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\old-site-projects\site_audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="URL History" sheetId="1" r:id="rId1"/>
@@ -1008,31 +1008,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1319,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
@@ -2124,12 +2100,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,7 +2256,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>165</v>
       </c>
@@ -2295,7 +2270,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>168</v>
       </c>
@@ -2309,7 +2284,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>177</v>
       </c>
@@ -2323,7 +2298,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>180</v>
       </c>
@@ -2337,7 +2312,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>189</v>
       </c>
@@ -2351,7 +2326,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>192</v>
       </c>
@@ -2365,7 +2340,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>213</v>
       </c>
@@ -2379,7 +2354,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>219</v>
       </c>
@@ -2393,7 +2368,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>222</v>
       </c>
@@ -2407,7 +2382,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>225</v>
       </c>
@@ -2421,7 +2396,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>228</v>
       </c>
@@ -2435,7 +2410,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>231</v>
       </c>
@@ -2449,7 +2424,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>234</v>
       </c>
@@ -2463,7 +2438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>243</v>
       </c>
@@ -2477,7 +2452,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>160</v>
       </c>
@@ -2489,7 +2464,7 @@
       </c>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>161</v>
       </c>
@@ -2501,7 +2476,7 @@
       </c>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>166</v>
       </c>
@@ -2513,7 +2488,7 @@
       </c>
       <c r="D31" s="9"/>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>169</v>
       </c>
@@ -2525,7 +2500,7 @@
       </c>
       <c r="D32" s="9"/>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>172</v>
       </c>
@@ -2537,7 +2512,7 @@
       </c>
       <c r="D33" s="9"/>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>161</v>
       </c>
@@ -2549,7 +2524,7 @@
       </c>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>175</v>
       </c>
@@ -2561,7 +2536,7 @@
       </c>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>198</v>
       </c>
@@ -2573,7 +2548,7 @@
       </c>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>201</v>
       </c>
@@ -2585,7 +2560,7 @@
       </c>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>204</v>
       </c>
@@ -2597,7 +2572,7 @@
       </c>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>207</v>
       </c>
@@ -2609,7 +2584,7 @@
       </c>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>210</v>
       </c>
@@ -2621,7 +2596,7 @@
       </c>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>216</v>
       </c>
@@ -2633,7 +2608,7 @@
       </c>
       <c r="D41" s="9"/>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>240</v>
       </c>
@@ -2645,7 +2620,7 @@
       </c>
       <c r="D42" s="9"/>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="9" t="s">
         <v>246</v>
@@ -2657,11 +2632,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A7:D43">
-    <filterColumn colId="0">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
     <sortState ref="A8:D43">
-      <sortCondition sortBy="cellColor" ref="A7:A43" dxfId="2"/>
+      <sortCondition sortBy="cellColor" ref="A7:A43" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>